<commit_message>
Update theory paper to include image of ray going up slope and timing tests, in preparation for publication to ASA.
</commit_message>
<xml_diff>
--- a/studies/cmp_speed/cmp_speed_test_20131104.xlsx
+++ b/studies/cmp_speed/cmp_speed_test_20131104.xlsx
@@ -117,26 +117,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Propagation Speed Test</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -148,6 +129,25 @@
           <c:tx>
             <c:v>CASS v4.2</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="12"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$12</c:f>
@@ -235,121 +235,8 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>WaveQ3D v0.3</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>5.16845</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.0543699999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.8017799999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.6484399999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.6123799999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.4384499999999996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.2689</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.023099999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11.8752</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12.4886</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>13.577500000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$D$1</c:f>
@@ -364,25 +251,19 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="12"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:marker>
@@ -504,11 +385,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116196864"/>
-        <c:axId val="116203520"/>
+        <c:axId val="110429696"/>
+        <c:axId val="110436352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116196864"/>
+        <c:axId val="110429696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -545,12 +426,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116203520"/>
+        <c:crossAx val="110436352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116203520"/>
+        <c:axId val="110436352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -587,7 +468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116196864"/>
+        <c:crossAx val="110429696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -595,15 +476,38 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21077186204861767"/>
+          <c:y val="0.23513246910854382"/>
+          <c:w val="0.18575042527787125"/>
+          <c:h val="0.10221700503381025"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:userShapes r:id="rId1"/>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
 </c:chartSpace>
 </file>
 
@@ -611,7 +515,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -622,7 +526,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662737" cy="6286500"/>
+    <xdr:ext cx="8676680" cy="6295430"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -643,197 +547,6 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.0926</cdr:x>
-      <cdr:y>0.10526</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.45081</cdr:x>
-      <cdr:y>0.40037</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="802128" y="661742"/>
-          <a:ext cx="3103157" cy="1855188"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>WaveQ3D version 0.4</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>Dell Latitude Laptop E6520</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>Intel i5-2540M CPU @2.60 GHz</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>calc time </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:sym typeface="Symbol"/>
-            </a:rPr>
-            <a:t></a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t> 8.47e-6 * R * D + 4.23e-2 * T</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>R = number of rays (181x25 = 4524)</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>D = propagation duration (80 sec)</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>T = number of targets</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.12153</cdr:x>
-      <cdr:y>0.70813</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.12153</cdr:x>
-      <cdr:y>0.85327</cdr:y>
-    </cdr:to>
-    <cdr:cxnSp macro="">
-      <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
-        <cdr:cNvCxnSpPr/>
-      </cdr:nvCxnSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1052763" y="4451684"/>
-          <a:ext cx="0" cy="912395"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </cdr:style>
-    </cdr:cxnSp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.09028</cdr:x>
-      <cdr:y>0.63796</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.19393</cdr:x>
-      <cdr:y>0.70744</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="5" name="TextBox 4"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="782030" y="4010513"/>
-          <a:ext cx="897938" cy="436786"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Crossover at</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>7 targets</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>